<commit_message>
Added docstrings to remainder of code
</commit_message>
<xml_diff>
--- a/test/mechanical/forecasts/ReportWeek2.xlsx
+++ b/test/mechanical/forecasts/ReportWeek2.xlsx
@@ -700,19 +700,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="11">
-        <v>0.263291367343765</v>
+        <v>0.2666644027248296</v>
       </c>
       <c r="C3" s="11"/>
       <c r="E3" s="11">
-        <v>0.5057489238611556</v>
+        <v>0.5065085892085137</v>
       </c>
       <c r="F3" s="11"/>
       <c r="H3" s="11">
-        <v>0.4137738998947945</v>
+        <v>0.4174682649269585</v>
       </c>
       <c r="I3" s="11"/>
       <c r="K3" s="11">
-        <v>0.7627585613100407</v>
+        <v>0.7656109038059924</v>
       </c>
       <c r="L3" s="11"/>
     </row>
@@ -721,19 +721,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="11">
-        <v>0.9131806738518395</v>
+        <v>0.9127915685431665</v>
       </c>
       <c r="C4" s="11"/>
       <c r="E4" s="11">
-        <v>0.9883674465155902</v>
+        <v>0.9883934056129343</v>
       </c>
       <c r="F4" s="11"/>
       <c r="H4" s="11">
-        <v>0.9906281334855674</v>
+        <v>0.9905827417658983</v>
       </c>
       <c r="I4" s="11"/>
       <c r="K4" s="11">
-        <v>0.9995591623406129</v>
+        <v>0.9995603030542934</v>
       </c>
       <c r="L4" s="11"/>
     </row>
@@ -742,19 +742,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="10">
-        <v>24.04325882503515</v>
+        <v>24.34090184378238</v>
       </c>
       <c r="C5" s="10"/>
       <c r="E5" s="10">
-        <v>49.9865772454658</v>
+        <v>50.06297494600056</v>
       </c>
       <c r="F5" s="10"/>
       <c r="H5" s="10">
-        <v>40.98960661378243</v>
+        <v>41.35368584715989</v>
       </c>
       <c r="I5" s="10"/>
       <c r="K5" s="10">
-        <v>76.24223086111954</v>
+        <v>76.52742670299892</v>
       </c>
       <c r="L5" s="10"/>
     </row>
@@ -763,28 +763,28 @@
         <v>4</v>
       </c>
       <c r="B6" s="12">
-        <v>0.3283006</v>
+        <v>0.3279243</v>
       </c>
       <c r="C6" s="12">
-        <v>0.6716993999999999</v>
+        <v>0.6720757000000001</v>
       </c>
       <c r="E6" s="12">
-        <v>0.4365911</v>
+        <v>0.4366617</v>
       </c>
       <c r="F6" s="12">
-        <v>0.5634089</v>
+        <v>0.5633383</v>
       </c>
       <c r="H6" s="12">
-        <v>0.4430702</v>
+        <v>0.4429328</v>
       </c>
       <c r="I6" s="12">
-        <v>0.5569298</v>
+        <v>0.5570672</v>
       </c>
       <c r="K6" s="12">
-        <v>0.4876401</v>
+        <v>0.4876561</v>
       </c>
       <c r="L6" s="12">
-        <v>0.5123599</v>
+        <v>0.5123439</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -792,28 +792,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="13">
-        <v>14.9962966</v>
+        <v>15.0019242</v>
       </c>
       <c r="C7" s="13">
-        <v>21.4901812</v>
+        <v>21.4999652</v>
       </c>
       <c r="E7" s="13">
-        <v>23.991193</v>
+        <v>23.99923</v>
       </c>
       <c r="F7" s="13">
-        <v>26.994349</v>
+        <v>27.0024572</v>
       </c>
       <c r="H7" s="13">
-        <v>28.8108116</v>
+        <v>28.8140564</v>
       </c>
       <c r="I7" s="13">
-        <v>31.5167234</v>
+        <v>31.5103236</v>
       </c>
       <c r="K7" s="13">
-        <v>24.9978058</v>
+        <v>25.000217</v>
       </c>
       <c r="L7" s="13">
-        <v>25.5084802</v>
+        <v>25.4994032</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1013,7 +1013,7 @@
         <v>25</v>
       </c>
       <c r="K14" s="13">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L14" s="13">
         <v>20</v>
@@ -1161,7 +1161,7 @@
         <v>27</v>
       </c>
       <c r="L19" s="13">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:12">

</xml_diff>